<commit_message>
increased bed size to 235mm
</commit_message>
<xml_diff>
--- a/Marlin Firmware Ender 3.xlsx
+++ b/Marlin Firmware Ender 3.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Marlin" sheetId="2" r:id="rId1"/>
     <sheet name="3DTouch" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Cura Start End code" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>marlin on ender 3</t>
   </si>
@@ -365,6 +366,81 @@
   </si>
   <si>
     <t>0       31      63      94      126     157     189     220</t>
+  </si>
+  <si>
+    <t>Cura Start and End code</t>
+  </si>
+  <si>
+    <t>; Ender 3 Custom Start G-code</t>
+  </si>
+  <si>
+    <t>G92 E0 ; Reset Extruder</t>
+  </si>
+  <si>
+    <t>G1 F1500 E-7 ; Retract filament 7 mm to prevent oozing</t>
+  </si>
+  <si>
+    <t>G28 ; Home all axes</t>
+  </si>
+  <si>
+    <t>M420 Z10 ; Leveling fade Z height</t>
+  </si>
+  <si>
+    <t>G29  ; BLTouch mesh generation</t>
+  </si>
+  <si>
+    <t>G1 Z5.0 F3000 ; Move Z Axis up little to prevent scratching of Heat Bed</t>
+  </si>
+  <si>
+    <t>G1 X0.1 Y20 Z0.3 F5000.0 ; Move to start position</t>
+  </si>
+  <si>
+    <t>G1 X0.1 Y200.0 Z0.2 F1500.0 E15 ; Draw the first line</t>
+  </si>
+  <si>
+    <t>G1 X0.4 Y200.0 Z0.2 F5000.0 ; Move to side a little</t>
+  </si>
+  <si>
+    <t>G1 X0.4 Y20 Z0.2 F1500.0 E30 ; Draw the second line</t>
+  </si>
+  <si>
+    <t>G1 Z2.0 F3000 ; Move Z Axis up little to prevent scratching of Heat Bed</t>
+  </si>
+  <si>
+    <t>; End of custom start GCode</t>
+  </si>
+  <si>
+    <t>; Ender 3 Custom End G-code</t>
+  </si>
+  <si>
+    <t>G4 ; Wait</t>
+  </si>
+  <si>
+    <t>M220 S100 ; Reset Speed factor override percentage to default (100%)</t>
+  </si>
+  <si>
+    <t>M221 S100 ; Reset Extrude factor override percentage to default (100%)</t>
+  </si>
+  <si>
+    <t>G91 ; Set coordinates to relative</t>
+  </si>
+  <si>
+    <t>G1 F1800 E-3 ; Retract filament 3 mm to prevent oozing</t>
+  </si>
+  <si>
+    <t>G1 F3000 Z20 ; Move Z Axis up 20 mm to allow filament ooze freely</t>
+  </si>
+  <si>
+    <t>G90 ; Set coordinates to absolute</t>
+  </si>
+  <si>
+    <t>G1 X0 Y{machine_depth} F1000 ; Move Heat Bed to the front for easy print removal</t>
+  </si>
+  <si>
+    <t>M84 ; Disable stepper motors</t>
+  </si>
+  <si>
+    <t>; End of custom end GCode</t>
   </si>
 </sst>
 </file>
@@ -1308,7 +1384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C15:N181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+    <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="L162" sqref="L162"/>
     </sheetView>
   </sheetViews>
@@ -1878,4 +1954,154 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:D35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>